<commit_message>
added estados, alertas and more
</commit_message>
<xml_diff>
--- a/docs/listado-productos.xlsx
+++ b/docs/listado-productos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repositorios\java2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repositorios\java2021\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE780831-3B39-47FA-B204-F80E7AE4A85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FF11E8-C15F-480E-8FFD-1575EB246E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5415" yWindow="2295" windowWidth="9420" windowHeight="10410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Shot Bloque Marron x35g</t>
+  </si>
+  <si>
+    <t>Cadbury Tableta x80g</t>
   </si>
 </sst>
 </file>
@@ -446,13 +449,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -488,10 +494,10 @@
         <v>80</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -508,10 +514,10 @@
         <v>80</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -528,10 +534,10 @@
         <v>80</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -548,10 +554,10 @@
         <v>80</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -568,10 +574,10 @@
         <v>80</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -588,10 +594,10 @@
         <v>40</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -608,10 +614,10 @@
         <v>40</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -628,10 +634,10 @@
         <v>40</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -648,10 +654,10 @@
         <v>40</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -668,10 +674,10 @@
         <v>40</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -688,10 +694,10 @@
         <v>40</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -708,10 +714,10 @@
         <v>40</v>
       </c>
       <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
         <v>3</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -728,10 +734,10 @@
         <v>40</v>
       </c>
       <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
         <v>3</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -748,10 +754,10 @@
         <v>40</v>
       </c>
       <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
         <v>3</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -765,13 +771,13 @@
         <v>95</v>
       </c>
       <c r="D16">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
         <v>4</v>
-      </c>
-      <c r="F16">
-        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -785,13 +791,13 @@
         <v>100</v>
       </c>
       <c r="D17">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
         <v>4</v>
-      </c>
-      <c r="F17">
-        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -808,10 +814,10 @@
         <v>250</v>
       </c>
       <c r="E18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -828,10 +834,10 @@
         <v>300</v>
       </c>
       <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
         <v>6</v>
-      </c>
-      <c r="F19">
-        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -848,10 +854,30 @@
         <v>100</v>
       </c>
       <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
         <v>6</v>
       </c>
-      <c r="F20">
-        <v>3</v>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21">
+        <v>300</v>
+      </c>
+      <c r="D21">
+        <v>125</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>